<commit_message>
Version submitted to PLDI 2012
</commit_message>
<xml_diff>
--- a/media/spreadsheets/OCamlComparison.xlsx
+++ b/media/spreadsheets/OCamlComparison.xlsx
@@ -45,22 +45,22 @@
     <t>C++</t>
   </si>
   <si>
-    <t>Tag/Spec</t>
-  </si>
-  <si>
-    <t>Tag/Uni</t>
-  </si>
-  <si>
-    <t>Kind/Spec</t>
-  </si>
-  <si>
     <t>OCaml</t>
   </si>
   <si>
-    <t>Open/Spec</t>
+    <t>Kind/Special</t>
   </si>
   <si>
-    <t>Open/Uni</t>
+    <t>Tag/Special</t>
+  </si>
+  <si>
+    <t>Tag/Unified</t>
+  </si>
+  <si>
+    <t>Open/Special</t>
+  </si>
+  <si>
+    <t>Open/Unifie</t>
   </si>
 </sst>
 </file>
@@ -278,19 +278,19 @@
                   <c:v>OCaml</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Kind/Spec</c:v>
+                  <c:v>Kind/Special</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Tag/Spec</c:v>
+                  <c:v>Tag/Special</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Tag/Uni</c:v>
+                  <c:v>Tag/Unified</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Open/Spec</c:v>
+                  <c:v>Open/Special</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Open/Uni</c:v>
+                  <c:v>Open/Unifie</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -332,11 +332,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="155449216"/>
-        <c:axId val="158818304"/>
+        <c:axId val="156232320"/>
+        <c:axId val="161693056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="155449216"/>
+        <c:axId val="156232320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -371,7 +371,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158818304"/>
+        <c:crossAx val="161693056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -379,7 +379,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158818304"/>
+        <c:axId val="161693056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,7 +416,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155449216"/>
+        <c:crossAx val="156232320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -591,19 +591,19 @@
                   <c:v>OCaml</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Kind/Spec</c:v>
+                  <c:v>Kind/Special</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Tag/Spec</c:v>
+                  <c:v>Tag/Special</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Tag/Uni</c:v>
+                  <c:v>Tag/Unified</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Open/Spec</c:v>
+                  <c:v>Open/Special</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Open/Uni</c:v>
+                  <c:v>Open/Unifie</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -645,11 +645,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="158841088"/>
-        <c:axId val="158855552"/>
+        <c:axId val="159570176"/>
+        <c:axId val="159719808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="158841088"/>
+        <c:axId val="159570176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -684,7 +684,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158855552"/>
+        <c:crossAx val="159719808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -692,7 +692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158855552"/>
+        <c:axId val="159719808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.000000000000001E-2"/>
@@ -730,7 +730,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158841088"/>
+        <c:crossAx val="159570176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -812,19 +812,19 @@
                   <c:v>OCaml</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Kind/Spec</c:v>
+                  <c:v>Kind/Special</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Tag/Spec</c:v>
+                  <c:v>Tag/Special</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Tag/Uni</c:v>
+                  <c:v>Tag/Unified</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Open/Spec</c:v>
+                  <c:v>Open/Special</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Open/Uni</c:v>
+                  <c:v>Open/Unifie</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -898,19 +898,19 @@
                   <c:v>OCaml</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Kind/Spec</c:v>
+                  <c:v>Kind/Special</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Tag/Spec</c:v>
+                  <c:v>Tag/Special</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Tag/Uni</c:v>
+                  <c:v>Tag/Unified</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Open/Spec</c:v>
+                  <c:v>Open/Special</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Open/Uni</c:v>
+                  <c:v>Open/Unifie</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -952,11 +952,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="76230016"/>
-        <c:axId val="103498880"/>
+        <c:axId val="159745920"/>
+        <c:axId val="159748096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76230016"/>
+        <c:axId val="159745920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -991,7 +991,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103498880"/>
+        <c:crossAx val="159748096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -999,7 +999,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103498880"/>
+        <c:axId val="159748096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,7 +1036,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76230016"/>
+        <c:crossAx val="159745920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1454,7 +1454,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,16 +1492,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>

</xml_diff>